<commit_message>
Adicionando a pagina inicial
</commit_message>
<xml_diff>
--- a/Artefactos/3. Proposta_Tecnica e Financeira/Plano_Negocio.xlsx
+++ b/Artefactos/3. Proposta_Tecnica e Financeira/Plano_Negocio.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="77">
   <si>
     <t>Designacao do Especialista</t>
   </si>
@@ -228,6 +228,24 @@
   </si>
   <si>
     <t>Total De Horas de Trabalho</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Divida</t>
+  </si>
+  <si>
+    <t>Executado</t>
+  </si>
+  <si>
+    <t>Falta</t>
   </si>
 </sst>
 </file>
@@ -235,9 +253,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,8 +277,15 @@
       <name val="Arial Black"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -284,6 +309,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -294,29 +331,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -325,18 +351,211 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="169" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="52">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF0070C0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -354,7 +573,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -362,7 +581,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -370,7 +589,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -378,7 +597,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -386,7 +605,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -394,7 +613,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -402,7 +621,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -410,7 +629,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -418,7 +637,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -426,7 +645,7 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="169" formatCode="#,##0.00\ [$MZM]"/>
+      <numFmt numFmtId="164" formatCode="#,##0.00\ [$MZM]"/>
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -455,12 +674,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="23"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="22"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="21">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="51"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="50"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="49">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="20">
+    <tableColumn id="10" name="Custo Total" dataDxfId="48">
       <calculatedColumnFormula>Table1[[#This Row],[Tempo em Hora]]*Table1[[#This Row],[Custo Por Hora]]*Table1[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -477,12 +696,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="19"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="18"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="17">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="47"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="46"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="45">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="16">
+    <tableColumn id="10" name="Custo Total" dataDxfId="44">
       <calculatedColumnFormula>Table14[[#This Row],[Tempo em Hora]]*Table14[[#This Row],[Custo Por Hora]]*Table14[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -499,12 +718,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="15"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="14"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="13">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="43"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="42"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="41">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="12">
+    <tableColumn id="10" name="Custo Total" dataDxfId="40">
       <calculatedColumnFormula>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -521,12 +740,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="11"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="10"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="9">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="39"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="38"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="37">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="8">
+    <tableColumn id="10" name="Custo Total" dataDxfId="36">
       <calculatedColumnFormula>Table1453[[#This Row],[Tempo em Hora]]*Table1453[[#This Row],[Custo Por Hora]]*Table1453[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -543,12 +762,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="7"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="6"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="5">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="35"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="34"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="33">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="4">
+    <tableColumn id="10" name="Custo Total" dataDxfId="32">
       <calculatedColumnFormula>Table14536[[#This Row],[Tempo em Hora]]*Table14536[[#This Row],[Custo Por Hora]]*Table14536[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -565,16 +784,16 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Total De Horas de Trabalho" dataDxfId="3">
+    <tableColumn id="3" name="Total De Horas de Trabalho" dataDxfId="31">
       <calculatedColumnFormula>SUM(SUMIF(Table14536[Designacao do Especialista],C53,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C53,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C53,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C53,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C53,Table1[Tempo em Hora]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Custo Por Hora" dataDxfId="0">
+    <tableColumn id="5" name="Custo Por Hora" dataDxfId="30">
       <calculatedColumnFormula>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Quantidade" dataDxfId="2">
+    <tableColumn id="9" name="Quantidade" dataDxfId="29">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="1">
+    <tableColumn id="10" name="Custo Total" dataDxfId="28">
       <calculatedColumnFormula>SUM(SUMIF(Table14536[Designacao do Especialista],C53,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C53,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C53,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C53,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C53,Table1[Custo Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -586,15 +805,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="C3:X28" totalsRowShown="0">
   <autoFilter ref="C3:X28"/>
   <tableColumns count="22">
-    <tableColumn id="1" name="codigo"/>
-    <tableColumn id="2" name="Processo"/>
-    <tableColumn id="3" name="1 Semana"/>
-    <tableColumn id="4" name="2 Semana"/>
-    <tableColumn id="5" name="3 Semana"/>
-    <tableColumn id="6" name="4 Semana"/>
-    <tableColumn id="7" name="5 Semana"/>
-    <tableColumn id="8" name="6 Semana"/>
-    <tableColumn id="9" name="7 Semana"/>
+    <tableColumn id="1" name="codigo" dataDxfId="27"/>
+    <tableColumn id="2" name="Processo" dataDxfId="26"/>
+    <tableColumn id="3" name="1 Semana" dataDxfId="25"/>
+    <tableColumn id="4" name="2 Semana" dataDxfId="24"/>
+    <tableColumn id="5" name="3 Semana" dataDxfId="23"/>
+    <tableColumn id="6" name="4 Semana" dataDxfId="22"/>
+    <tableColumn id="7" name="5 Semana" dataDxfId="21"/>
+    <tableColumn id="8" name="6 Semana" dataDxfId="20"/>
+    <tableColumn id="9" name="7 Semana" dataDxfId="19"/>
     <tableColumn id="10" name="8 Semana"/>
     <tableColumn id="11" name="9 Semana"/>
     <tableColumn id="12" name="10 Semana"/>
@@ -903,29 +1122,29 @@
   <dimension ref="B3:H62"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
-      <selection activeCell="B51" sqref="B51:G62"/>
+      <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="2" max="2" width="8.5234375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39.1015625" customWidth="1"/>
-    <col min="4" max="4" width="14.734375" style="8" customWidth="1"/>
-    <col min="5" max="5" width="15.3671875" style="9" customWidth="1"/>
-    <col min="6" max="6" width="8.5234375" style="10" customWidth="1"/>
-    <col min="7" max="7" width="25.26171875" style="9" customWidth="1"/>
+    <col min="4" max="4" width="14.734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="15.3671875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="8.5234375" style="4" customWidth="1"/>
+    <col min="7" max="7" width="25.26171875" style="3" customWidth="1"/>
     <col min="8" max="8" width="12.20703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
+      <c r="C3" s="9"/>
+      <c r="D3" s="9"/>
+      <c r="E3" s="9"/>
+      <c r="F3" s="9"/>
+      <c r="G3" s="9"/>
     </row>
     <row r="4" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -934,16 +1153,16 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="D4" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F4" s="10" t="s">
+      <c r="F4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G4" s="9" t="s">
+      <c r="G4" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -954,16 +1173,16 @@
       <c r="C5" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="2">
         <v>30</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="3">
         <v>0</v>
       </c>
-      <c r="F5" s="8">
-        <v>1</v>
-      </c>
-      <c r="G5" s="9">
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3">
         <f>Table1[[#This Row],[Tempo em Hora]]*Table1[[#This Row],[Custo Por Hora]]*Table1[[#This Row],[Quantidade]]</f>
         <v>0</v>
       </c>
@@ -975,16 +1194,16 @@
       <c r="C6" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="2">
         <v>30</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="3">
         <v>200</v>
       </c>
-      <c r="F6" s="8">
-        <v>1</v>
-      </c>
-      <c r="G6" s="9">
+      <c r="F6" s="2">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3">
         <f>Table1[[#This Row],[Tempo em Hora]]*Table1[[#This Row],[Custo Por Hora]]*Table1[[#This Row],[Quantidade]]</f>
         <v>6000</v>
       </c>
@@ -996,54 +1215,54 @@
       <c r="C7" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="2">
         <v>30</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="3">
         <v>500</v>
       </c>
-      <c r="F7" s="8">
-        <v>1</v>
-      </c>
-      <c r="G7" s="9">
+      <c r="F7" s="2">
+        <v>1</v>
+      </c>
+      <c r="G7" s="3">
         <f>Table1[[#This Row],[Tempo em Hora]]*Table1[[#This Row],[Custo Por Hora]]*Table1[[#This Row],[Quantidade]]</f>
         <v>15000</v>
       </c>
     </row>
     <row r="8" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="7"/>
-      <c r="D8" s="11">
+      <c r="C8" s="10"/>
+      <c r="D8" s="5">
         <f>SUM(Table1[Tempo em Hora])</f>
         <v>90</v>
       </c>
-      <c r="E8" s="12">
+      <c r="E8" s="6">
         <f>SUM(Table1[Custo Por Hora])</f>
         <v>700</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="7">
         <f>SUM(Table1[Quantidade])</f>
         <v>3</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="6">
         <f>SUM(Table1[Custo Total])</f>
         <v>21000</v>
       </c>
     </row>
     <row r="9" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="F9" s="8"/>
+      <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="2"/>
+      <c r="C10" s="9"/>
+      <c r="D10" s="9"/>
+      <c r="E10" s="9"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -1052,16 +1271,16 @@
       <c r="C11" t="s">
         <v>0</v>
       </c>
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E11" s="9" t="s">
+      <c r="E11" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F11" s="10" t="s">
+      <c r="F11" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1072,16 +1291,16 @@
       <c r="C12" t="s">
         <v>5</v>
       </c>
-      <c r="D12" s="8">
+      <c r="D12" s="2">
         <v>30</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="3">
         <v>0</v>
       </c>
-      <c r="F12" s="8">
-        <v>1</v>
-      </c>
-      <c r="G12" s="9">
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="3">
         <f>Table14[[#This Row],[Tempo em Hora]]*Table14[[#This Row],[Custo Por Hora]]*Table14[[#This Row],[Quantidade]]</f>
         <v>0</v>
       </c>
@@ -1093,16 +1312,16 @@
       <c r="C13" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="2">
         <v>240</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="3">
         <v>200</v>
       </c>
-      <c r="F13" s="8">
-        <v>1</v>
-      </c>
-      <c r="G13" s="9">
+      <c r="F13" s="2">
+        <v>1</v>
+      </c>
+      <c r="G13" s="3">
         <f>Table14[[#This Row],[Tempo em Hora]]*Table14[[#This Row],[Custo Por Hora]]*Table14[[#This Row],[Quantidade]]</f>
         <v>48000</v>
       </c>
@@ -1114,16 +1333,16 @@
       <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="2">
         <v>240</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="3">
         <v>500</v>
       </c>
-      <c r="F14" s="8">
-        <v>1</v>
-      </c>
-      <c r="G14" s="9">
+      <c r="F14" s="2">
+        <v>1</v>
+      </c>
+      <c r="G14" s="3">
         <f>Table14[[#This Row],[Tempo em Hora]]*Table14[[#This Row],[Custo Por Hora]]*Table14[[#This Row],[Quantidade]]</f>
         <v>120000</v>
       </c>
@@ -1135,16 +1354,16 @@
       <c r="C15" t="s">
         <v>7</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="2">
         <v>240</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="3">
         <v>400</v>
       </c>
-      <c r="F15" s="8">
-        <v>1</v>
-      </c>
-      <c r="G15" s="9">
+      <c r="F15" s="2">
+        <v>1</v>
+      </c>
+      <c r="G15" s="3">
         <f>Table14[[#This Row],[Tempo em Hora]]*Table14[[#This Row],[Custo Por Hora]]*Table14[[#This Row],[Quantidade]]</f>
         <v>96000</v>
       </c>
@@ -1156,54 +1375,54 @@
       <c r="C16" t="s">
         <v>8</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="2">
         <v>240</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="3">
         <v>200</v>
       </c>
-      <c r="F16" s="8">
+      <c r="F16" s="2">
         <v>2</v>
       </c>
-      <c r="G16" s="9">
+      <c r="G16" s="3">
         <f>Table14[[#This Row],[Tempo em Hora]]*Table14[[#This Row],[Custo Por Hora]]*Table14[[#This Row],[Quantidade]]</f>
         <v>96000</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B17" s="7" t="s">
+      <c r="B17" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="7"/>
-      <c r="D17" s="11">
+      <c r="C17" s="10"/>
+      <c r="D17" s="5">
         <f>SUM(Table14[Tempo em Hora])</f>
         <v>990</v>
       </c>
-      <c r="E17" s="12">
+      <c r="E17" s="6">
         <f>SUM(Table14[Custo Por Hora])</f>
         <v>1300</v>
       </c>
-      <c r="F17" s="13">
+      <c r="F17" s="7">
         <f>SUM(Table14[Quantidade])</f>
         <v>6</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="6">
         <f>SUM(Table14[Custo Total])</f>
         <v>360000</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="F19" s="8"/>
+      <c r="F19" s="2"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="1" t="s">
+      <c r="B20" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
@@ -1212,16 +1431,16 @@
       <c r="C21" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="8" t="s">
+      <c r="D21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E21" s="9" t="s">
+      <c r="E21" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G21" s="9" t="s">
+      <c r="G21" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1232,16 +1451,16 @@
       <c r="C22" t="s">
         <v>6</v>
       </c>
-      <c r="D22" s="8">
+      <c r="D22" s="2">
         <v>88</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E22" s="3">
         <v>200</v>
       </c>
-      <c r="F22" s="8">
-        <v>1</v>
-      </c>
-      <c r="G22" s="9">
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="3">
         <f>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</f>
         <v>17600</v>
       </c>
@@ -1253,16 +1472,16 @@
       <c r="C23" t="s">
         <v>8</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D23" s="2">
         <v>200</v>
       </c>
-      <c r="E23" s="9">
+      <c r="E23" s="3">
         <v>200</v>
       </c>
-      <c r="F23" s="8">
+      <c r="F23" s="2">
         <v>2</v>
       </c>
-      <c r="G23" s="9">
+      <c r="G23" s="3">
         <f>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</f>
         <v>80000</v>
       </c>
@@ -1274,16 +1493,16 @@
       <c r="C24" t="s">
         <v>7</v>
       </c>
-      <c r="D24" s="8">
+      <c r="D24" s="2">
         <v>150</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="3">
         <v>400</v>
       </c>
-      <c r="F24" s="8">
-        <v>1</v>
-      </c>
-      <c r="G24" s="9">
+      <c r="F24" s="2">
+        <v>1</v>
+      </c>
+      <c r="G24" s="3">
         <f>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</f>
         <v>60000</v>
       </c>
@@ -1295,16 +1514,16 @@
       <c r="C25" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="8">
+      <c r="D25" s="2">
         <v>200</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="3">
         <v>150</v>
       </c>
-      <c r="F25" s="8">
-        <v>1</v>
-      </c>
-      <c r="G25" s="9">
+      <c r="F25" s="2">
+        <v>1</v>
+      </c>
+      <c r="G25" s="3">
         <f>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</f>
         <v>30000</v>
       </c>
@@ -1316,16 +1535,16 @@
       <c r="C26" t="s">
         <v>65</v>
       </c>
-      <c r="D26" s="8">
+      <c r="D26" s="2">
         <v>100</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="3">
         <v>200</v>
       </c>
-      <c r="F26" s="8">
-        <v>1</v>
-      </c>
-      <c r="G26" s="9">
+      <c r="F26" s="2">
+        <v>1</v>
+      </c>
+      <c r="G26" s="3">
         <f>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</f>
         <v>20000</v>
       </c>
@@ -1337,16 +1556,16 @@
       <c r="C27" t="s">
         <v>13</v>
       </c>
-      <c r="D27" s="8">
+      <c r="D27" s="2">
         <v>440</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="3">
         <v>500</v>
       </c>
-      <c r="F27" s="8">
-        <v>1</v>
-      </c>
-      <c r="G27" s="9">
+      <c r="F27" s="2">
+        <v>1</v>
+      </c>
+      <c r="G27" s="3">
         <f>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</f>
         <v>220000</v>
       </c>
@@ -1358,16 +1577,16 @@
       <c r="C28" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="8">
+      <c r="D28" s="2">
         <v>440</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="3">
         <v>200</v>
       </c>
-      <c r="F28" s="8">
-        <v>1</v>
-      </c>
-      <c r="G28" s="9">
+      <c r="F28" s="2">
+        <v>1</v>
+      </c>
+      <c r="G28" s="3">
         <f>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</f>
         <v>88000</v>
       </c>
@@ -1379,51 +1598,51 @@
       <c r="C29" t="s">
         <v>68</v>
       </c>
-      <c r="D29" s="8">
+      <c r="D29" s="2">
         <v>440</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="3">
         <v>100</v>
       </c>
-      <c r="F29" s="8">
+      <c r="F29" s="2">
         <v>5</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="3">
         <f>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</f>
         <v>220000</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B30" s="7" t="s">
+      <c r="B30" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="7"/>
-      <c r="D30" s="11">
+      <c r="C30" s="10"/>
+      <c r="D30" s="5">
         <f>SUM(Table145[Tempo em Hora])</f>
         <v>2058</v>
       </c>
-      <c r="E30" s="12">
+      <c r="E30" s="6">
         <f>SUM(Table145[Custo Por Hora])</f>
         <v>1950</v>
       </c>
-      <c r="F30" s="13">
+      <c r="F30" s="7">
         <f>SUM(Table145[Quantidade])</f>
         <v>13</v>
       </c>
-      <c r="G30" s="12">
+      <c r="G30" s="6">
         <f>SUM(Table145[Custo Total])</f>
         <v>735600</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="1" t="s">
+      <c r="B32" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="2"/>
-      <c r="D32" s="2"/>
-      <c r="E32" s="2"/>
-      <c r="F32" s="2"/>
-      <c r="G32" s="2"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
@@ -1432,16 +1651,16 @@
       <c r="C33" t="s">
         <v>0</v>
       </c>
-      <c r="D33" s="8" t="s">
+      <c r="D33" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E33" s="9" t="s">
+      <c r="E33" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G33" s="9" t="s">
+      <c r="G33" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1452,16 +1671,16 @@
       <c r="C34" t="s">
         <v>6</v>
       </c>
-      <c r="D34" s="8">
+      <c r="D34" s="2">
         <v>50</v>
       </c>
-      <c r="E34" s="9">
+      <c r="E34" s="3">
         <v>200</v>
       </c>
-      <c r="F34" s="8">
-        <v>1</v>
-      </c>
-      <c r="G34" s="9">
+      <c r="F34" s="2">
+        <v>1</v>
+      </c>
+      <c r="G34" s="3">
         <f>Table1453[[#This Row],[Tempo em Hora]]*Table1453[[#This Row],[Custo Por Hora]]*Table1453[[#This Row],[Quantidade]]</f>
         <v>10000</v>
       </c>
@@ -1473,16 +1692,16 @@
       <c r="C35" t="s">
         <v>8</v>
       </c>
-      <c r="D35" s="8">
+      <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="9">
+      <c r="E35" s="3">
         <v>200</v>
       </c>
-      <c r="F35" s="8">
-        <v>1</v>
-      </c>
-      <c r="G35" s="9">
+      <c r="F35" s="2">
+        <v>1</v>
+      </c>
+      <c r="G35" s="3">
         <f>Table1453[[#This Row],[Tempo em Hora]]*Table1453[[#This Row],[Custo Por Hora]]*Table1453[[#This Row],[Quantidade]]</f>
         <v>10000</v>
       </c>
@@ -1494,16 +1713,16 @@
       <c r="C36" t="s">
         <v>7</v>
       </c>
-      <c r="D36" s="8">
+      <c r="D36" s="2">
         <v>50</v>
       </c>
-      <c r="E36" s="9">
+      <c r="E36" s="3">
         <v>400</v>
       </c>
-      <c r="F36" s="8">
-        <v>1</v>
-      </c>
-      <c r="G36" s="9">
+      <c r="F36" s="2">
+        <v>1</v>
+      </c>
+      <c r="G36" s="3">
         <f>Table1453[[#This Row],[Tempo em Hora]]*Table1453[[#This Row],[Custo Por Hora]]*Table1453[[#This Row],[Quantidade]]</f>
         <v>20000</v>
       </c>
@@ -1515,16 +1734,16 @@
       <c r="C37" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="8">
+      <c r="D37" s="2">
         <v>50</v>
       </c>
-      <c r="E37" s="9">
+      <c r="E37" s="3">
         <v>0</v>
       </c>
-      <c r="F37" s="8">
-        <v>1</v>
-      </c>
-      <c r="G37" s="9">
+      <c r="F37" s="2">
+        <v>1</v>
+      </c>
+      <c r="G37" s="3">
         <f>Table1453[[#This Row],[Tempo em Hora]]*Table1453[[#This Row],[Custo Por Hora]]*Table1453[[#This Row],[Quantidade]]</f>
         <v>0</v>
       </c>
@@ -1536,51 +1755,51 @@
       <c r="C38" t="s">
         <v>13</v>
       </c>
-      <c r="D38" s="8">
+      <c r="D38" s="2">
         <v>50</v>
       </c>
-      <c r="E38" s="9">
+      <c r="E38" s="3">
         <v>500</v>
       </c>
-      <c r="F38" s="8">
-        <v>1</v>
-      </c>
-      <c r="G38" s="9">
+      <c r="F38" s="2">
+        <v>1</v>
+      </c>
+      <c r="G38" s="3">
         <f>Table1453[[#This Row],[Tempo em Hora]]*Table1453[[#This Row],[Custo Por Hora]]*Table1453[[#This Row],[Quantidade]]</f>
         <v>25000</v>
       </c>
     </row>
     <row r="39" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B39" s="7" t="s">
+      <c r="B39" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="7"/>
-      <c r="D39" s="11">
+      <c r="C39" s="10"/>
+      <c r="D39" s="5">
         <f>SUM(Table1453[Tempo em Hora])</f>
         <v>250</v>
       </c>
-      <c r="E39" s="12">
+      <c r="E39" s="6">
         <f>SUM(Table1453[Custo Por Hora])</f>
         <v>1300</v>
       </c>
-      <c r="F39" s="13">
+      <c r="F39" s="7">
         <f>SUM(Table1453[Quantidade])</f>
         <v>5</v>
       </c>
-      <c r="G39" s="12">
+      <c r="G39" s="6">
         <f>SUM(Table1453[Custo Total])</f>
         <v>65000</v>
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="2"/>
+      <c r="C42" s="9"/>
+      <c r="D42" s="9"/>
+      <c r="E42" s="9"/>
+      <c r="F42" s="9"/>
+      <c r="G42" s="9"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
@@ -1589,16 +1808,16 @@
       <c r="C43" t="s">
         <v>0</v>
       </c>
-      <c r="D43" s="8" t="s">
+      <c r="D43" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E43" s="9" t="s">
+      <c r="E43" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F43" s="10" t="s">
+      <c r="F43" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G43" s="9" t="s">
+      <c r="G43" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1609,16 +1828,16 @@
       <c r="C44" t="s">
         <v>8</v>
       </c>
-      <c r="D44" s="8">
+      <c r="D44" s="2">
         <v>40</v>
       </c>
-      <c r="E44" s="9">
+      <c r="E44" s="3">
         <v>200</v>
       </c>
-      <c r="F44" s="8">
-        <v>1</v>
-      </c>
-      <c r="G44" s="9">
+      <c r="F44" s="2">
+        <v>1</v>
+      </c>
+      <c r="G44" s="3">
         <f>Table14536[[#This Row],[Tempo em Hora]]*Table14536[[#This Row],[Custo Por Hora]]*Table14536[[#This Row],[Quantidade]]</f>
         <v>8000</v>
       </c>
@@ -1630,16 +1849,16 @@
       <c r="C45" t="s">
         <v>7</v>
       </c>
-      <c r="D45" s="8">
+      <c r="D45" s="2">
         <v>40</v>
       </c>
-      <c r="E45" s="9">
+      <c r="E45" s="3">
         <v>400</v>
       </c>
-      <c r="F45" s="8">
-        <v>1</v>
-      </c>
-      <c r="G45" s="9">
+      <c r="F45" s="2">
+        <v>1</v>
+      </c>
+      <c r="G45" s="3">
         <f>Table14536[[#This Row],[Tempo em Hora]]*Table14536[[#This Row],[Custo Por Hora]]*Table14536[[#This Row],[Quantidade]]</f>
         <v>16000</v>
       </c>
@@ -1651,16 +1870,16 @@
       <c r="C46" t="s">
         <v>5</v>
       </c>
-      <c r="D46" s="8">
+      <c r="D46" s="2">
         <v>40</v>
       </c>
-      <c r="E46" s="9">
+      <c r="E46" s="3">
         <v>0</v>
       </c>
-      <c r="F46" s="8">
-        <v>1</v>
-      </c>
-      <c r="G46" s="9">
+      <c r="F46" s="2">
+        <v>1</v>
+      </c>
+      <c r="G46" s="3">
         <f>Table14536[[#This Row],[Tempo em Hora]]*Table14536[[#This Row],[Custo Por Hora]]*Table14536[[#This Row],[Quantidade]]</f>
         <v>0</v>
       </c>
@@ -1672,51 +1891,51 @@
       <c r="C47" t="s">
         <v>13</v>
       </c>
-      <c r="D47" s="8">
+      <c r="D47" s="2">
         <v>40</v>
       </c>
-      <c r="E47" s="9">
+      <c r="E47" s="3">
         <v>500</v>
       </c>
-      <c r="F47" s="8">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
+      <c r="F47" s="2">
+        <v>1</v>
+      </c>
+      <c r="G47" s="3">
         <f>Table14536[[#This Row],[Tempo em Hora]]*Table14536[[#This Row],[Custo Por Hora]]*Table14536[[#This Row],[Quantidade]]</f>
         <v>20000</v>
       </c>
     </row>
     <row r="48" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B48" s="7" t="s">
+      <c r="B48" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="7"/>
-      <c r="D48" s="11">
+      <c r="C48" s="10"/>
+      <c r="D48" s="5">
         <f>SUM(Table14536[Tempo em Hora])</f>
         <v>160</v>
       </c>
-      <c r="E48" s="12">
+      <c r="E48" s="6">
         <f>SUM(Table14536[Custo Por Hora])</f>
         <v>1100</v>
       </c>
-      <c r="F48" s="13">
+      <c r="F48" s="7">
         <f>SUM(Table14536[Quantidade])</f>
         <v>4</v>
       </c>
-      <c r="G48" s="12">
+      <c r="G48" s="6">
         <f>SUM(Table14536[Custo Total])</f>
         <v>44000</v>
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="1" t="s">
+      <c r="B51" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="9"/>
+      <c r="G51" s="9"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" t="s">
@@ -1725,16 +1944,16 @@
       <c r="C52" t="s">
         <v>0</v>
       </c>
-      <c r="D52" s="8" t="s">
+      <c r="D52" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E52" s="8" t="s">
+      <c r="E52" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F52" s="10" t="s">
+      <c r="F52" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="G52" s="9" t="s">
+      <c r="G52" s="3" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1745,18 +1964,18 @@
       <c r="C53" t="s">
         <v>66</v>
       </c>
-      <c r="D53" s="8">
+      <c r="D53" s="2">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C53,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C53,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C53,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C53,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C53,Table1[Tempo em Hora]))</f>
         <v>200</v>
       </c>
-      <c r="E53" s="8">
+      <c r="E53" s="2">
         <f>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</f>
         <v>150</v>
       </c>
-      <c r="F53" s="8">
-        <v>1</v>
-      </c>
-      <c r="G53" s="9">
+      <c r="F53" s="2">
+        <v>1</v>
+      </c>
+      <c r="G53" s="3">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C53,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C53,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C53,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C53,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C53,Table1[Custo Total]))</f>
         <v>30000</v>
       </c>
@@ -1768,18 +1987,18 @@
       <c r="C54" t="s">
         <v>65</v>
       </c>
-      <c r="D54" s="8">
+      <c r="D54" s="2">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C54,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C54,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C54,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C54,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C54,Table1[Tempo em Hora]))</f>
         <v>100</v>
       </c>
-      <c r="E54" s="8">
+      <c r="E54" s="2">
         <f>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</f>
         <v>200</v>
       </c>
-      <c r="F54" s="8">
-        <v>1</v>
-      </c>
-      <c r="G54" s="9">
+      <c r="F54" s="2">
+        <v>1</v>
+      </c>
+      <c r="G54" s="3">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C54,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C54,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C54,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C54,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C54,Table1[Custo Total]))</f>
         <v>20000</v>
       </c>
@@ -1791,18 +2010,18 @@
       <c r="C55" t="s">
         <v>6</v>
       </c>
-      <c r="D55" s="8">
+      <c r="D55" s="2">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C55,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C55,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C55,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C55,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C55,Table1[Tempo em Hora]))</f>
         <v>408</v>
       </c>
-      <c r="E55" s="8">
+      <c r="E55" s="2">
         <f>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</f>
         <v>200</v>
       </c>
-      <c r="F55" s="8">
-        <v>1</v>
-      </c>
-      <c r="G55" s="9">
+      <c r="F55" s="2">
+        <v>1</v>
+      </c>
+      <c r="G55" s="3">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C55,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C55,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C55,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C55,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C55,Table1[Custo Total]))</f>
         <v>81600</v>
       </c>
@@ -1814,18 +2033,18 @@
       <c r="C56" t="s">
         <v>8</v>
       </c>
-      <c r="D56" s="8">
+      <c r="D56" s="2">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C56,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C56,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C56,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C56,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C56,Table1[Tempo em Hora]))</f>
         <v>530</v>
       </c>
-      <c r="E56" s="8">
+      <c r="E56" s="2">
         <f>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</f>
         <v>366.03773584905662</v>
       </c>
-      <c r="F56" s="8">
+      <c r="F56" s="2">
         <v>2</v>
       </c>
-      <c r="G56" s="9">
+      <c r="G56" s="3">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C56,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C56,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C56,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C56,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C56,Table1[Custo Total]))</f>
         <v>194000</v>
       </c>
@@ -1837,18 +2056,18 @@
       <c r="C57" t="s">
         <v>7</v>
       </c>
-      <c r="D57" s="8">
+      <c r="D57" s="2">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C57,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C57,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C57,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C57,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C57,Table1[Tempo em Hora]))</f>
         <v>480</v>
       </c>
-      <c r="E57" s="8">
+      <c r="E57" s="2">
         <f>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</f>
         <v>400</v>
       </c>
-      <c r="F57" s="8">
-        <v>1</v>
-      </c>
-      <c r="G57" s="9">
+      <c r="F57" s="2">
+        <v>1</v>
+      </c>
+      <c r="G57" s="3">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C57,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C57,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C57,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C57,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C57,Table1[Custo Total]))</f>
         <v>192000</v>
       </c>
@@ -1860,18 +2079,18 @@
       <c r="C58" t="s">
         <v>5</v>
       </c>
-      <c r="D58" s="8">
+      <c r="D58" s="2">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C58,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C58,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C58,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C58,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C58,Table1[Tempo em Hora]))</f>
         <v>150</v>
       </c>
-      <c r="E58" s="8">
+      <c r="E58" s="2">
         <f>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</f>
         <v>0</v>
       </c>
-      <c r="F58" s="8">
-        <v>1</v>
-      </c>
-      <c r="G58" s="9">
+      <c r="F58" s="2">
+        <v>1</v>
+      </c>
+      <c r="G58" s="3">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C58,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C58,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C58,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C58,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C58,Table1[Custo Total]))</f>
         <v>0</v>
       </c>
@@ -1883,18 +2102,18 @@
       <c r="C59" t="s">
         <v>13</v>
       </c>
-      <c r="D59" s="8">
+      <c r="D59" s="2">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C59,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C59,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C59,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C59,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C59,Table1[Tempo em Hora]))</f>
         <v>800</v>
       </c>
-      <c r="E59" s="8">
+      <c r="E59" s="2">
         <f>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</f>
         <v>500</v>
       </c>
-      <c r="F59" s="8">
-        <v>1</v>
-      </c>
-      <c r="G59" s="9">
+      <c r="F59" s="2">
+        <v>1</v>
+      </c>
+      <c r="G59" s="3">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C59,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C59,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C59,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C59,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C59,Table1[Custo Total]))</f>
         <v>400000</v>
       </c>
@@ -1906,18 +2125,18 @@
       <c r="C60" t="s">
         <v>68</v>
       </c>
-      <c r="D60" s="8">
+      <c r="D60" s="2">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C60,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C60,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C60,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C60,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C60,Table1[Tempo em Hora]))</f>
         <v>440</v>
       </c>
-      <c r="E60" s="8">
+      <c r="E60" s="2">
         <f>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</f>
         <v>500</v>
       </c>
-      <c r="F60" s="8">
+      <c r="F60" s="2">
         <v>5</v>
       </c>
-      <c r="G60" s="9">
+      <c r="G60" s="3">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C60,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C60,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C60,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C60,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C60,Table1[Custo Total]))</f>
         <v>220000</v>
       </c>
@@ -1929,47 +2148,52 @@
       <c r="C61" t="s">
         <v>67</v>
       </c>
-      <c r="D61" s="8">
+      <c r="D61" s="2">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C61,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C61,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C61,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C61,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C61,Table1[Tempo em Hora]))</f>
         <v>440</v>
       </c>
-      <c r="E61" s="8">
+      <c r="E61" s="2">
         <f>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</f>
         <v>200</v>
       </c>
-      <c r="F61" s="8">
-        <v>1</v>
-      </c>
-      <c r="G61" s="9">
+      <c r="F61" s="2">
+        <v>1</v>
+      </c>
+      <c r="G61" s="3">
         <f>SUM(SUMIF(Table14536[Designacao do Especialista],C61,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C61,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C61,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C61,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C61,Table1[Custo Total]))</f>
         <v>88000</v>
       </c>
     </row>
     <row r="62" spans="2:8" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B62" s="7" t="s">
+      <c r="B62" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="7"/>
-      <c r="D62" s="11">
+      <c r="C62" s="10"/>
+      <c r="D62" s="5">
         <f>SUM(Table145368[Total De Horas de Trabalho])</f>
         <v>3548</v>
       </c>
-      <c r="E62" s="11">
+      <c r="E62" s="5">
         <f>SUM(Table145368[Custo Por Hora])</f>
         <v>2516.0377358490568</v>
       </c>
-      <c r="F62" s="13">
+      <c r="F62" s="7">
         <f>SUM(Table145368[Quantidade])</f>
         <v>14</v>
       </c>
-      <c r="G62" s="12">
+      <c r="G62" s="6">
         <f>SUM(Table145368[Custo Total])</f>
         <v>1225600</v>
       </c>
-      <c r="H62" s="6"/>
+      <c r="H62" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B3:G3"/>
+    <mergeCell ref="B10:G10"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="B20:G20"/>
     <mergeCell ref="B51:G51"/>
     <mergeCell ref="B62:C62"/>
     <mergeCell ref="B30:C30"/>
@@ -1977,11 +2201,6 @@
     <mergeCell ref="B39:C39"/>
     <mergeCell ref="B42:G42"/>
     <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B3:G3"/>
-    <mergeCell ref="B10:G10"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="B20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1998,35 +2217,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C1:X28"/>
+  <dimension ref="C1:X35"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="W27" sqref="W27"/>
+    <sheetView topLeftCell="C3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="4" max="4" width="38.3671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="10" width="10.734375" hidden="1" customWidth="1"/>
-    <col min="11" max="13" width="10.734375" customWidth="1"/>
+    <col min="3" max="3" width="8.83984375" style="14"/>
+    <col min="4" max="4" width="38.3671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="13" width="10.734375" customWidth="1"/>
     <col min="14" max="20" width="11.734375" customWidth="1"/>
     <col min="21" max="22" width="11.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="3" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C3" t="s">
+      <c r="C3" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="14" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
@@ -2091,278 +2310,472 @@
       </c>
     </row>
     <row r="4" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4">
-        <v>1</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="C4" s="14">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="3"/>
+      <c r="E4" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
     </row>
     <row r="5" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5">
+      <c r="C5" s="14">
         <v>2</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="3"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
     </row>
     <row r="6" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6">
+      <c r="C6" s="14">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G6" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
     </row>
     <row r="7" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7">
+      <c r="C7" s="14">
         <v>4</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="G7" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
     </row>
     <row r="8" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C8">
+      <c r="C8" s="14">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H8" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
     </row>
     <row r="9" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C9">
+      <c r="C9" s="14">
         <v>6</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="12"/>
+      <c r="G9" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="11"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
     </row>
     <row r="10" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C10">
+      <c r="C10" s="14">
         <v>7</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I10" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
     </row>
     <row r="11" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C11">
+      <c r="C11" s="14">
         <v>8</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12"/>
+      <c r="G11" s="12"/>
+      <c r="H11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
     </row>
     <row r="12" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C12">
+      <c r="C12" s="14">
         <v>9</v>
       </c>
-      <c r="D12" t="s">
+      <c r="D12" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="12"/>
+      <c r="G12" s="12"/>
+      <c r="H12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="11"/>
     </row>
     <row r="13" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C13">
+      <c r="C13" s="14">
         <v>10</v>
       </c>
-      <c r="D13" t="s">
+      <c r="D13" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="12"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
+      <c r="I13" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="11"/>
     </row>
     <row r="14" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C14">
+      <c r="C14" s="14">
         <v>11</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D14" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="F14" s="4"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15">
+      <c r="E14" s="11"/>
+      <c r="F14" s="12"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
+      <c r="I14" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="11"/>
+    </row>
+    <row r="15" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" s="14">
         <v>12</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D15" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-    </row>
-    <row r="16" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C16">
+      <c r="F15" s="12"/>
+      <c r="G15" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="I15" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="J15" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" s="14">
         <v>13</v>
       </c>
-      <c r="D16" t="s">
+      <c r="D16" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17">
+      <c r="F16" s="12"/>
+      <c r="K16" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="17" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="14">
         <v>14</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="F17" s="4"/>
-      <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
-    </row>
-    <row r="18" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18">
+      <c r="F17" s="12"/>
+      <c r="L17" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="M17" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" s="14">
         <v>15</v>
       </c>
-      <c r="D18" t="s">
+      <c r="D18" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="N18" s="3"/>
-    </row>
-    <row r="19" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19">
+      <c r="N18" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="19" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19" s="14">
         <v>16</v>
       </c>
-      <c r="D19" t="s">
+      <c r="D19" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="M19" s="4"/>
-      <c r="N19" s="3"/>
-      <c r="O19" s="3"/>
-    </row>
-    <row r="20" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C20">
+      <c r="M19" s="12"/>
+      <c r="N19" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="O19" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20" s="14">
         <v>17</v>
       </c>
-      <c r="D20" t="s">
+      <c r="D20" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="P20" s="3"/>
-    </row>
-    <row r="21" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C21">
+      <c r="P20" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="21" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21" s="14">
         <v>18</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D21" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="P21" s="3"/>
-      <c r="Q21" s="3"/>
-    </row>
-    <row r="22" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C22">
+      <c r="P21" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q21" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C22" s="14">
         <v>19</v>
       </c>
-      <c r="D22" t="s">
+      <c r="D22" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="R22" s="3"/>
-    </row>
-    <row r="23" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C23">
+      <c r="R22" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="23" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C23" s="14">
         <v>20</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="R23" s="3"/>
-      <c r="S23" s="3"/>
-      <c r="T23" s="4"/>
-      <c r="U23" s="4"/>
-      <c r="V23" s="4"/>
-      <c r="W23" s="4"/>
-      <c r="X23" s="4"/>
-    </row>
-    <row r="24" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C24">
+      <c r="R23" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="S23" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="T23" s="12"/>
+      <c r="U23" s="12"/>
+      <c r="V23" s="12"/>
+      <c r="W23" s="12"/>
+      <c r="X23" s="12"/>
+    </row>
+    <row r="24" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C24" s="14">
         <v>21</v>
       </c>
-      <c r="D24" t="s">
+      <c r="D24" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="T24" s="3"/>
-    </row>
-    <row r="25" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C25">
+      <c r="T24" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="25" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C25" s="14">
         <v>22</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D25" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="T25" s="3"/>
-      <c r="U25" s="3"/>
-      <c r="V25" s="4"/>
-      <c r="W25" s="4"/>
-      <c r="X25" s="4"/>
-    </row>
-    <row r="26" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C26">
+      <c r="T25" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="U25" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="V25" s="12"/>
+      <c r="W25" s="12"/>
+      <c r="X25" s="12"/>
+    </row>
+    <row r="26" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C26" s="14">
         <v>23</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D26" s="14" t="s">
         <v>59</v>
       </c>
-      <c r="V26" s="3"/>
-      <c r="W26" s="4"/>
-      <c r="X26" s="4"/>
-    </row>
-    <row r="27" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27">
+      <c r="V26" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="W26" s="12"/>
+      <c r="X26" s="12"/>
+    </row>
+    <row r="27" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C27" s="14">
         <v>24</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="W27" s="3"/>
-      <c r="X27" s="4"/>
-    </row>
-    <row r="28" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28">
+      <c r="W27" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="X27" s="12"/>
+    </row>
+    <row r="28" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C28" s="14">
         <v>25</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="X28" s="3"/>
+      <c r="X28" s="13" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="3:24" hidden="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="E31">
+        <f>COUNTA(Table6[[1 Semana]:[20 Semana]])</f>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C33" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="D33" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E33" s="16">
+        <f>COUNTIF(Table6[[1 Semana]:[20 Semana]],"X")/E31</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="34" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C34" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D34" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="E34" s="16">
+        <f>COUNTIF(Table6[[1 Semana]:[20 Semana]],"D")/E31</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="35" spans="3:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="C35" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>76</v>
+      </c>
+      <c r="E35" s="16">
+        <f>COUNTIF(Table6[[1 Semana]:[20 Semana]],"D")/E31</f>
+        <v>0.25</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="J1:N1"/>
   </mergeCells>
+  <conditionalFormatting sqref="E1:X33 E35:X1048576 E34:G34 I34:X34">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+      <formula>"D"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+      <formula>"X"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4:X28">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"x"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+      <formula>"F"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <tableParts count="1">

</xml_diff>

<commit_message>
Adicionando o Plano de Gerenciamento de Mudancas
</commit_message>
<xml_diff>
--- a/Artefactos/3. Proposta_Tecnica e Financeira/Plano_Negocio.xlsx
+++ b/Artefactos/3. Proposta_Tecnica e Financeira/Plano_Negocio.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="452"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" tabRatio="452" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Custo de Pessoal" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="78">
   <si>
     <t>Designacao do Especialista</t>
   </si>
@@ -246,6 +246,9 @@
   </si>
   <si>
     <t>Falta</t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -357,13 +360,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -389,13 +385,54 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="38">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -413,27 +450,6 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FF0070C0"/>
         </patternFill>
       </fill>
@@ -444,117 +460,6 @@
           <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF0070C0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -674,12 +579,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="51"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="50"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="49">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="37"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="36"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="35">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="48">
+    <tableColumn id="10" name="Custo Total" dataDxfId="34">
       <calculatedColumnFormula>Table1[[#This Row],[Tempo em Hora]]*Table1[[#This Row],[Custo Por Hora]]*Table1[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -696,12 +601,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="47"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="46"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="45">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="33"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="32"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="31">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="44">
+    <tableColumn id="10" name="Custo Total" dataDxfId="30">
       <calculatedColumnFormula>Table14[[#This Row],[Tempo em Hora]]*Table14[[#This Row],[Custo Por Hora]]*Table14[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -718,12 +623,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="43"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="42"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="41">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="29"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="28"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="27">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="40">
+    <tableColumn id="10" name="Custo Total" dataDxfId="26">
       <calculatedColumnFormula>Table145[[#This Row],[Tempo em Hora]]*Table145[[#This Row],[Custo Por Hora]]*Table145[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -740,12 +645,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="39"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="38"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="37">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="25"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="24"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="23">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="36">
+    <tableColumn id="10" name="Custo Total" dataDxfId="22">
       <calculatedColumnFormula>Table1453[[#This Row],[Tempo em Hora]]*Table1453[[#This Row],[Custo Por Hora]]*Table1453[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -762,12 +667,12 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Tempo em Hora" dataDxfId="35"/>
-    <tableColumn id="4" name="Custo Por Hora" dataDxfId="34"/>
-    <tableColumn id="9" name="Quantidade" dataDxfId="33">
+    <tableColumn id="3" name="Tempo em Hora" dataDxfId="21"/>
+    <tableColumn id="4" name="Custo Por Hora" dataDxfId="20"/>
+    <tableColumn id="9" name="Quantidade" dataDxfId="19">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="32">
+    <tableColumn id="10" name="Custo Total" dataDxfId="18">
       <calculatedColumnFormula>Table14536[[#This Row],[Tempo em Hora]]*Table14536[[#This Row],[Custo Por Hora]]*Table14536[[#This Row],[Quantidade]]</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -784,16 +689,16 @@
   <tableColumns count="6">
     <tableColumn id="1" name="Codigo"/>
     <tableColumn id="2" name="Designacao do Especialista"/>
-    <tableColumn id="3" name="Total De Horas de Trabalho" dataDxfId="31">
+    <tableColumn id="3" name="Total De Horas de Trabalho" dataDxfId="17">
       <calculatedColumnFormula>SUM(SUMIF(Table14536[Designacao do Especialista],C53,Table14536[Tempo em Hora]),SUMIF(Table1453[Designacao do Especialista],C53,Table1453[Tempo em Hora]),SUMIF(Table145[Designacao do Especialista],C53,Table145[Tempo em Hora]),SUMIF(Table14[Designacao do Especialista],C53,Table14[Tempo em Hora]),SUMIF(Table1[Designacao do Especialista],C53,Table1[Tempo em Hora]))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="5" name="Custo Por Hora" dataDxfId="30">
+    <tableColumn id="5" name="Custo Por Hora" dataDxfId="16">
       <calculatedColumnFormula>Table145368[[#This Row],[Custo Total]]/Table145368[[#This Row],[Total De Horas de Trabalho]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" name="Quantidade" dataDxfId="29">
+    <tableColumn id="9" name="Quantidade" dataDxfId="15">
       <calculatedColumnFormula>SUM(#REF!)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" name="Custo Total" dataDxfId="28">
+    <tableColumn id="10" name="Custo Total" dataDxfId="14">
       <calculatedColumnFormula>SUM(SUMIF(Table14536[Designacao do Especialista],C53,Table14536[Custo Total]),SUMIF(Table1453[Designacao do Especialista],C53,Table1453[Custo Total]),SUMIF(Table145[Designacao do Especialista],C53,Table145[Custo Total]),SUMIF(Table14[Designacao do Especialista],C53,Table14[Custo Total]),SUMIF(Table1[Designacao do Especialista],C53,Table1[Custo Total]))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -805,15 +710,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="C3:X28" totalsRowShown="0">
   <autoFilter ref="C3:X28"/>
   <tableColumns count="22">
-    <tableColumn id="1" name="codigo" dataDxfId="27"/>
-    <tableColumn id="2" name="Processo" dataDxfId="26"/>
-    <tableColumn id="3" name="1 Semana" dataDxfId="25"/>
-    <tableColumn id="4" name="2 Semana" dataDxfId="24"/>
-    <tableColumn id="5" name="3 Semana" dataDxfId="23"/>
-    <tableColumn id="6" name="4 Semana" dataDxfId="22"/>
-    <tableColumn id="7" name="5 Semana" dataDxfId="21"/>
-    <tableColumn id="8" name="6 Semana" dataDxfId="20"/>
-    <tableColumn id="9" name="7 Semana" dataDxfId="19"/>
+    <tableColumn id="1" name="codigo" dataDxfId="8"/>
+    <tableColumn id="2" name="Processo" dataDxfId="7"/>
+    <tableColumn id="3" name="1 Semana" dataDxfId="6"/>
+    <tableColumn id="4" name="2 Semana" dataDxfId="5"/>
+    <tableColumn id="5" name="3 Semana" dataDxfId="4"/>
+    <tableColumn id="6" name="4 Semana" dataDxfId="3"/>
+    <tableColumn id="7" name="5 Semana" dataDxfId="2"/>
+    <tableColumn id="8" name="6 Semana" dataDxfId="1"/>
+    <tableColumn id="9" name="7 Semana" dataDxfId="0"/>
     <tableColumn id="10" name="8 Semana"/>
     <tableColumn id="11" name="9 Semana"/>
     <tableColumn id="12" name="10 Semana"/>
@@ -1121,7 +1026,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:H62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView topLeftCell="A38" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="E56" sqref="E56"/>
     </sheetView>
   </sheetViews>
@@ -1137,14 +1042,14 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="9"/>
-      <c r="D3" s="9"/>
-      <c r="E3" s="9"/>
-      <c r="F3" s="9"/>
-      <c r="G3" s="9"/>
+      <c r="C3" s="18"/>
+      <c r="D3" s="18"/>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
     </row>
     <row r="4" spans="2:7" ht="19.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
@@ -1230,10 +1135,10 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="10"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="5">
         <f>SUM(Table1[Tempo em Hora])</f>
         <v>90</v>
@@ -1255,14 +1160,14 @@
       <c r="F9" s="2"/>
     </row>
     <row r="10" spans="2:7" x14ac:dyDescent="0.3">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
-      <c r="E10" s="9"/>
-      <c r="F10" s="9"/>
-      <c r="G10" s="9"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
     </row>
     <row r="11" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
@@ -1390,10 +1295,10 @@
       </c>
     </row>
     <row r="17" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B17" s="10" t="s">
+      <c r="B17" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="10"/>
+      <c r="C17" s="19"/>
       <c r="D17" s="5">
         <f>SUM(Table14[Tempo em Hora])</f>
         <v>990</v>
@@ -1415,14 +1320,14 @@
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="9"/>
-      <c r="F20" s="9"/>
-      <c r="G20" s="9"/>
+      <c r="C20" s="18"/>
+      <c r="D20" s="18"/>
+      <c r="E20" s="18"/>
+      <c r="F20" s="18"/>
+      <c r="G20" s="18"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B21" t="s">
@@ -1613,10 +1518,10 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B30" s="10" t="s">
+      <c r="B30" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C30" s="10"/>
+      <c r="C30" s="19"/>
       <c r="D30" s="5">
         <f>SUM(Table145[Tempo em Hora])</f>
         <v>2058</v>
@@ -1635,14 +1540,14 @@
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="17" t="s">
         <v>15</v>
       </c>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9"/>
-      <c r="E32" s="9"/>
-      <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
+      <c r="C32" s="18"/>
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+      <c r="F32" s="18"/>
+      <c r="G32" s="18"/>
     </row>
     <row r="33" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
@@ -1770,10 +1675,10 @@
       </c>
     </row>
     <row r="39" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C39" s="10"/>
+      <c r="C39" s="19"/>
       <c r="D39" s="5">
         <f>SUM(Table1453[Tempo em Hora])</f>
         <v>250</v>
@@ -1792,14 +1697,14 @@
       </c>
     </row>
     <row r="42" spans="2:7" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42" s="8" t="s">
+      <c r="B42" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="9"/>
-      <c r="D42" s="9"/>
-      <c r="E42" s="9"/>
-      <c r="F42" s="9"/>
-      <c r="G42" s="9"/>
+      <c r="C42" s="18"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="18"/>
+      <c r="F42" s="18"/>
+      <c r="G42" s="18"/>
     </row>
     <row r="43" spans="2:7" x14ac:dyDescent="0.3">
       <c r="B43" t="s">
@@ -1884,7 +1789,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="2:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:7" x14ac:dyDescent="0.55000000000000004">
       <c r="B47">
         <v>4</v>
       </c>
@@ -1906,10 +1811,10 @@
       </c>
     </row>
     <row r="48" spans="2:7" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B48" s="10" t="s">
+      <c r="B48" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C48" s="10"/>
+      <c r="C48" s="19"/>
       <c r="D48" s="5">
         <f>SUM(Table14536[Tempo em Hora])</f>
         <v>160</v>
@@ -1928,14 +1833,14 @@
       </c>
     </row>
     <row r="51" spans="2:8" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51" s="8" t="s">
+      <c r="B51" s="17" t="s">
         <v>69</v>
       </c>
-      <c r="C51" s="9"/>
-      <c r="D51" s="9"/>
-      <c r="E51" s="9"/>
-      <c r="F51" s="9"/>
-      <c r="G51" s="9"/>
+      <c r="C51" s="18"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
     </row>
     <row r="52" spans="2:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" t="s">
@@ -2165,10 +2070,10 @@
       </c>
     </row>
     <row r="62" spans="2:8" ht="17.100000000000001" x14ac:dyDescent="0.8">
-      <c r="B62" s="10" t="s">
+      <c r="B62" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="C62" s="10"/>
+      <c r="C62" s="19"/>
       <c r="D62" s="5">
         <f>SUM(Table145368[Total De Horas de Trabalho])</f>
         <v>3548</v>
@@ -2219,33 +2124,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C1:X35"/>
   <sheetViews>
-    <sheetView topLeftCell="C3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="P20" sqref="P20"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="8.83984375" style="14"/>
-    <col min="4" max="4" width="38.3671875" style="14" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.83984375" style="11"/>
+    <col min="4" max="4" width="38.3671875" style="11" bestFit="1" customWidth="1"/>
     <col min="5" max="13" width="10.734375" customWidth="1"/>
     <col min="14" max="20" width="11.734375" customWidth="1"/>
     <col min="21" max="22" width="11.734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="3" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="11" t="s">
         <v>17</v>
       </c>
       <c r="E3" t="s">
@@ -2310,404 +2215,404 @@
       </c>
     </row>
     <row r="4" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C4" s="14">
-        <v>1</v>
-      </c>
-      <c r="D4" s="14" t="s">
+      <c r="C4" s="11">
+        <v>1</v>
+      </c>
+      <c r="D4" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="H4" s="11"/>
-      <c r="I4" s="11"/>
-      <c r="J4" s="11"/>
-      <c r="K4" s="11"/>
+      <c r="F4" s="8"/>
+      <c r="G4" s="8"/>
+      <c r="H4" s="8"/>
+      <c r="I4" s="8"/>
+      <c r="J4" s="8"/>
+      <c r="K4" s="8"/>
     </row>
     <row r="5" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C5" s="14">
+      <c r="C5" s="11">
         <v>2</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="10"/>
+      <c r="F5" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="G5" s="8" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
+    </row>
+    <row r="6" spans="3:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="C6" s="11">
+        <v>3</v>
+      </c>
+      <c r="D6" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="8"/>
+      <c r="F6" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="11"/>
-      <c r="J5" s="11"/>
-      <c r="K5" s="11"/>
-    </row>
-    <row r="6" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C6" s="14">
-        <v>3</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="E6" s="11"/>
-      <c r="F6" s="13" t="s">
+      <c r="G6" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G6" s="13" t="s">
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+    </row>
+    <row r="7" spans="3:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="C7" s="11">
+        <v>4</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E7" s="8"/>
+      <c r="F7" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="H6" s="11"/>
-      <c r="I6" s="11"/>
-      <c r="J6" s="11"/>
-      <c r="K6" s="11"/>
-    </row>
-    <row r="7" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C7" s="14">
-        <v>4</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="E7" s="11"/>
-      <c r="F7" s="13" t="s">
+      <c r="G7" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G7" s="13" t="s">
+      <c r="H7" s="8"/>
+      <c r="I7" s="8"/>
+      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
+    </row>
+    <row r="8" spans="3:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="C8" s="11">
+        <v>5</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="8"/>
+      <c r="F8" s="9"/>
+      <c r="G8" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
-      <c r="J7" s="11"/>
-      <c r="K7" s="11"/>
-    </row>
-    <row r="8" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C8" s="14">
-        <v>5</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="13" t="s">
+      <c r="H8" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="H8" s="13" t="s">
+      <c r="I8" s="8"/>
+      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
+    </row>
+    <row r="9" spans="3:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="C9" s="11">
+        <v>6</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" s="8"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
+      <c r="K9" s="8"/>
+    </row>
+    <row r="10" spans="3:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="C10" s="11">
+        <v>7</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" s="8"/>
+      <c r="F10" s="9"/>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
+    </row>
+    <row r="11" spans="3:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="C11" s="11">
+        <v>8</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I11" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
+    </row>
+    <row r="12" spans="3:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="C12" s="11">
+        <v>9</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="8"/>
+      <c r="F12" s="9"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K12" s="8"/>
+    </row>
+    <row r="13" spans="3:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="C13" s="11">
+        <v>10</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="8"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="8"/>
+      <c r="I13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K13" s="8"/>
+    </row>
+    <row r="14" spans="3:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="C14" s="11">
+        <v>11</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="E14" s="8"/>
+      <c r="F14" s="9"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="I8" s="11"/>
-      <c r="J8" s="11"/>
-      <c r="K8" s="11"/>
-    </row>
-    <row r="9" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C9" s="14">
-        <v>6</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="E9" s="11"/>
-      <c r="F9" s="12"/>
-      <c r="G9" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="H9" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I9" s="11"/>
-      <c r="J9" s="11"/>
-      <c r="K9" s="11"/>
-    </row>
-    <row r="10" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C10" s="14">
-        <v>7</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10" s="11"/>
-      <c r="F10" s="12"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I10" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="J10" s="11"/>
-      <c r="K10" s="11"/>
-    </row>
-    <row r="11" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C11" s="14">
-        <v>8</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12"/>
-      <c r="G11" s="12"/>
-      <c r="H11" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I11" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11"/>
-    </row>
-    <row r="12" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C12" s="14">
-        <v>9</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="11"/>
-      <c r="F12" s="12"/>
-      <c r="G12" s="12"/>
-      <c r="H12" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="K12" s="11"/>
-    </row>
-    <row r="13" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C13" s="14">
-        <v>10</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="E13" s="11"/>
-      <c r="F13" s="12"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>72</v>
-      </c>
-      <c r="K13" s="11"/>
-    </row>
-    <row r="14" spans="3:24" x14ac:dyDescent="0.55000000000000004">
-      <c r="C14" s="14">
-        <v>11</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="11"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="11"/>
-      <c r="H14" s="11"/>
-      <c r="I14" s="13" t="s">
+      <c r="J14" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="13" t="s">
+      <c r="K14" s="8"/>
+    </row>
+    <row r="15" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C15" s="11">
+        <v>12</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="F15" s="9"/>
+      <c r="G15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="K14" s="11"/>
-    </row>
-    <row r="15" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C15" s="14">
-        <v>12</v>
-      </c>
-      <c r="D15" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F15" s="12"/>
-      <c r="G15" s="13" t="s">
+      <c r="H15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="13" t="s">
+      <c r="I15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="13" t="s">
+      <c r="J15" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="13" t="s">
+    </row>
+    <row r="16" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C16" s="11">
+        <v>13</v>
+      </c>
+      <c r="D16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="K16" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="16" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C16" s="14">
-        <v>13</v>
-      </c>
-      <c r="D16" s="14" t="s">
-        <v>41</v>
-      </c>
-      <c r="F16" s="12"/>
-      <c r="K16" s="13" t="s">
+    <row r="17" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C17" s="11">
+        <v>14</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="9"/>
+      <c r="L17" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="17" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C17" s="14">
-        <v>14</v>
-      </c>
-      <c r="D17" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="F17" s="12"/>
-      <c r="L17" s="13" t="s">
+      <c r="M17" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="M17" s="13" t="s">
+    </row>
+    <row r="18" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C18" s="11">
+        <v>15</v>
+      </c>
+      <c r="D18" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="N18" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="18" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C18" s="14">
-        <v>15</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="N18" s="13" t="s">
+    <row r="19" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C19" s="11">
+        <v>16</v>
+      </c>
+      <c r="D19" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="M19" s="9"/>
+      <c r="N19" s="10" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="19" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C19" s="14">
-        <v>16</v>
-      </c>
-      <c r="D19" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="M19" s="12"/>
-      <c r="N19" s="13" t="s">
+      <c r="O19" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="O19" s="13" t="s">
+    </row>
+    <row r="20" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C20" s="11">
+        <v>17</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="P20" s="10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C20" s="14">
-        <v>17</v>
-      </c>
-      <c r="D20" s="14" t="s">
-        <v>56</v>
-      </c>
-      <c r="P20" s="13" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="21" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C21" s="14">
+    <row r="21" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C21" s="11">
         <v>18</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="P21" s="13" t="s">
+      <c r="P21" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="Q21" s="13" t="s">
+      <c r="Q21" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="22" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C22" s="14">
+    <row r="22" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C22" s="11">
         <v>19</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="R22" s="13" t="s">
+      <c r="R22" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C23" s="14">
+    <row r="23" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C23" s="11">
         <v>20</v>
       </c>
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R23" s="13" t="s">
+      <c r="R23" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="S23" s="13" t="s">
+      <c r="S23" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="T23" s="12"/>
-      <c r="U23" s="12"/>
-      <c r="V23" s="12"/>
-      <c r="W23" s="12"/>
-      <c r="X23" s="12"/>
-    </row>
-    <row r="24" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C24" s="14">
+      <c r="T23" s="9"/>
+      <c r="U23" s="9"/>
+      <c r="V23" s="9"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="9"/>
+    </row>
+    <row r="24" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C24" s="11">
         <v>21</v>
       </c>
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="T24" s="13" t="s">
+      <c r="T24" s="10" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="25" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C25" s="14">
+    <row r="25" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C25" s="11">
         <v>22</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="T25" s="13" t="s">
+      <c r="T25" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="U25" s="13" t="s">
+      <c r="U25" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="V25" s="12"/>
-      <c r="W25" s="12"/>
-      <c r="X25" s="12"/>
-    </row>
-    <row r="26" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C26" s="14">
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+    </row>
+    <row r="26" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C26" s="11">
         <v>23</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="V26" s="13" t="s">
+      <c r="V26" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="W26" s="12"/>
-      <c r="X26" s="12"/>
-    </row>
-    <row r="27" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C27" s="14">
+      <c r="W26" s="9"/>
+      <c r="X26" s="9"/>
+    </row>
+    <row r="27" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C27" s="11">
         <v>24</v>
       </c>
-      <c r="D27" s="15" t="s">
+      <c r="D27" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="W27" s="13" t="s">
+      <c r="W27" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="X27" s="12"/>
-    </row>
-    <row r="28" spans="3:24" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="C28" s="14">
+      <c r="X27" s="9"/>
+    </row>
+    <row r="28" spans="3:24" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="C28" s="11">
         <v>25</v>
       </c>
-      <c r="D28" s="15" t="s">
+      <c r="D28" s="12" t="s">
         <v>62</v>
       </c>
-      <c r="X28" s="13" t="s">
+      <c r="X28" s="10" t="s">
         <v>73</v>
       </c>
     </row>
@@ -2718,39 +2623,39 @@
       </c>
     </row>
     <row r="33" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C33" s="14" t="s">
+      <c r="C33" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E33" s="16">
+      <c r="E33" s="13">
         <f>COUNTIF(Table6[[1 Semana]:[20 Semana]],"X")/E31</f>
-        <v>0.5</v>
+        <v>0.54545454545454541</v>
       </c>
     </row>
     <row r="34" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C34" s="14" t="s">
+      <c r="C34" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D34" s="17" t="s">
+      <c r="D34" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="E34" s="16">
+      <c r="E34" s="13">
         <f>COUNTIF(Table6[[1 Semana]:[20 Semana]],"D")/E31</f>
-        <v>0.25</v>
+        <v>0.20454545454545456</v>
       </c>
     </row>
     <row r="35" spans="3:5" x14ac:dyDescent="0.55000000000000004">
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="D35" s="19" t="s">
+      <c r="D35" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="E35" s="16">
+      <c r="E35" s="13">
         <f>COUNTIF(Table6[[1 Semana]:[20 Semana]],"D")/E31</f>
-        <v>0.25</v>
+        <v>0.20454545454545456</v>
       </c>
     </row>
   </sheetData>
@@ -2758,21 +2663,21 @@
     <mergeCell ref="J1:N1"/>
   </mergeCells>
   <conditionalFormatting sqref="E1:X33 E35:X1048576 E34:G34 I34:X34">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="equal">
       <formula>"D"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"X"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:X28">
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="equal">
       <formula>"F"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="equal">
       <formula>"x"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="equal">
       <formula>"F"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>